<commit_message>
Operand refactor and flow control
</commit_message>
<xml_diff>
--- a/doc/ISA.xlsx
+++ b/doc/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\RISC-16\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B71E5C9-7DE1-46D1-80B5-13E9F0ADD9C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA8AD06-0C8E-4B2D-B420-EF88E54EB57F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A8037CD1-89C4-49B2-BEBC-F011A8AA52CE}"/>
   </bookViews>
@@ -219,7 +219,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +229,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0C1FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,22 +386,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,6 +560,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE0C1FF"/>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -856,7 +877,7 @@
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,84 +893,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="18"/>
       <c r="Q1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="17" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+      <c r="A2" s="15">
         <v>15</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="15">
         <v>14</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="15">
         <v>13</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="15">
         <v>12</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="15">
         <v>11</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="15">
         <v>10</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="15">
         <v>9</v>
       </c>
-      <c r="H2" s="17">
-        <v>8</v>
-      </c>
-      <c r="I2" s="17">
+      <c r="H2" s="15">
+        <v>8</v>
+      </c>
+      <c r="I2" s="15">
         <v>7</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="15">
         <v>6</v>
       </c>
-      <c r="K2" s="17">
+      <c r="K2" s="15">
         <v>5</v>
       </c>
-      <c r="L2" s="17">
-        <v>4</v>
-      </c>
-      <c r="M2" s="17">
+      <c r="L2" s="15">
+        <v>4</v>
+      </c>
+      <c r="M2" s="15">
         <v>3</v>
       </c>
-      <c r="N2" s="17">
+      <c r="N2" s="15">
         <v>2</v>
       </c>
-      <c r="O2" s="17">
-        <v>1</v>
-      </c>
-      <c r="P2" s="18">
+      <c r="O2" s="15">
+        <v>1</v>
+      </c>
+      <c r="P2" s="16">
         <v>0</v>
       </c>
       <c r="Q2" s="20"/>
-      <c r="R2" s="15"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -976,28 +997,28 @@
       <c r="H3" s="8">
         <v>0</v>
       </c>
-      <c r="I3" s="9">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
-        <v>0</v>
-      </c>
-      <c r="O3" s="8">
-        <v>0</v>
-      </c>
-      <c r="P3" s="10">
+      <c r="I3" s="21">
+        <v>0</v>
+      </c>
+      <c r="J3" s="22">
+        <v>0</v>
+      </c>
+      <c r="K3" s="22">
+        <v>0</v>
+      </c>
+      <c r="L3" s="22">
+        <v>0</v>
+      </c>
+      <c r="M3" s="22">
+        <v>0</v>
+      </c>
+      <c r="N3" s="22">
+        <v>0</v>
+      </c>
+      <c r="O3" s="22">
+        <v>0</v>
+      </c>
+      <c r="P3" s="23">
         <v>0</v>
       </c>
       <c r="Q3" s="1" t="s">
@@ -1032,28 +1053,28 @@
       <c r="H4" s="8">
         <v>0</v>
       </c>
-      <c r="I4" s="8">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8">
-        <v>0</v>
-      </c>
-      <c r="L4" s="8">
-        <v>0</v>
-      </c>
-      <c r="M4" s="8">
-        <v>0</v>
-      </c>
-      <c r="N4" s="8">
-        <v>0</v>
-      </c>
-      <c r="O4" s="8">
-        <v>0</v>
-      </c>
-      <c r="P4" s="10">
+      <c r="I4" s="22">
+        <v>0</v>
+      </c>
+      <c r="J4" s="22">
+        <v>0</v>
+      </c>
+      <c r="K4" s="22">
+        <v>0</v>
+      </c>
+      <c r="L4" s="22">
+        <v>0</v>
+      </c>
+      <c r="M4" s="22">
+        <v>0</v>
+      </c>
+      <c r="N4" s="22">
+        <v>0</v>
+      </c>
+      <c r="O4" s="22">
+        <v>0</v>
+      </c>
+      <c r="P4" s="23">
         <v>1</v>
       </c>
       <c r="Q4" s="1" t="s">
@@ -1092,16 +1113,16 @@
       <c r="C6" s="8">
         <v>0</v>
       </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8">
+      <c r="D6" s="22">
+        <v>0</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0</v>
+      </c>
+      <c r="G6" s="22">
         <v>0</v>
       </c>
       <c r="H6" s="8" t="s">
@@ -1148,16 +1169,16 @@
       <c r="C7" s="8">
         <v>0</v>
       </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8">
+      <c r="D7" s="22">
+        <v>0</v>
+      </c>
+      <c r="E7" s="22">
+        <v>0</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0</v>
+      </c>
+      <c r="G7" s="22">
         <v>1</v>
       </c>
       <c r="H7" s="8" t="s">
@@ -1204,16 +1225,16 @@
       <c r="C8" s="8">
         <v>0</v>
       </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8">
+      <c r="D8" s="22">
+        <v>0</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0</v>
+      </c>
+      <c r="F8" s="22">
+        <v>1</v>
+      </c>
+      <c r="G8" s="22">
         <v>0</v>
       </c>
       <c r="H8" s="8" t="s">
@@ -1260,16 +1281,16 @@
       <c r="C9" s="8">
         <v>0</v>
       </c>
-      <c r="D9" s="8">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8">
-        <v>1</v>
-      </c>
-      <c r="G9" s="8">
+      <c r="D9" s="22">
+        <v>0</v>
+      </c>
+      <c r="E9" s="22">
+        <v>0</v>
+      </c>
+      <c r="F9" s="22">
+        <v>1</v>
+      </c>
+      <c r="G9" s="22">
         <v>1</v>
       </c>
       <c r="H9" s="8" t="s">
@@ -1316,16 +1337,16 @@
       <c r="C10" s="8">
         <v>0</v>
       </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8">
+      <c r="D10" s="22">
+        <v>0</v>
+      </c>
+      <c r="E10" s="22">
+        <v>1</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0</v>
+      </c>
+      <c r="G10" s="22">
         <v>0</v>
       </c>
       <c r="H10" s="8" t="s">
@@ -1372,16 +1393,16 @@
       <c r="C11" s="8">
         <v>0</v>
       </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <v>1</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
+      <c r="D11" s="22">
+        <v>0</v>
+      </c>
+      <c r="E11" s="22">
+        <v>1</v>
+      </c>
+      <c r="F11" s="22">
+        <v>0</v>
+      </c>
+      <c r="G11" s="22">
         <v>1</v>
       </c>
       <c r="H11" s="8" t="s">
@@ -1428,16 +1449,16 @@
       <c r="C12" s="8">
         <v>0</v>
       </c>
-      <c r="D12" s="8">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8">
+      <c r="D12" s="22">
+        <v>0</v>
+      </c>
+      <c r="E12" s="22">
+        <v>1</v>
+      </c>
+      <c r="F12" s="22">
+        <v>1</v>
+      </c>
+      <c r="G12" s="22">
         <v>0</v>
       </c>
       <c r="H12" s="8" t="s">
@@ -1484,16 +1505,16 @@
       <c r="C13" s="8">
         <v>0</v>
       </c>
-      <c r="D13" s="8">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
-        <v>1</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8">
+      <c r="D13" s="22">
+        <v>0</v>
+      </c>
+      <c r="E13" s="22">
+        <v>1</v>
+      </c>
+      <c r="F13" s="22">
+        <v>1</v>
+      </c>
+      <c r="G13" s="22">
         <v>1</v>
       </c>
       <c r="H13" s="8" t="s">
@@ -1540,16 +1561,16 @@
       <c r="C14" s="8">
         <v>0</v>
       </c>
-      <c r="D14" s="8">
-        <v>1</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8">
+      <c r="D14" s="22">
+        <v>1</v>
+      </c>
+      <c r="E14" s="22">
+        <v>0</v>
+      </c>
+      <c r="F14" s="22">
+        <v>0</v>
+      </c>
+      <c r="G14" s="22">
         <v>0</v>
       </c>
       <c r="H14" s="8" t="s">
@@ -1615,10 +1636,10 @@
       <c r="C16" s="8">
         <v>1</v>
       </c>
-      <c r="D16" s="8">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="D16" s="22">
+        <v>0</v>
+      </c>
+      <c r="E16" s="22">
         <v>0</v>
       </c>
       <c r="F16" s="8" t="s">
@@ -1671,10 +1692,10 @@
       <c r="C17" s="8">
         <v>1</v>
       </c>
-      <c r="D17" s="8">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8">
+      <c r="D17" s="22">
+        <v>0</v>
+      </c>
+      <c r="E17" s="22">
         <v>1</v>
       </c>
       <c r="F17" s="8" t="s">
@@ -1743,22 +1764,22 @@
       <c r="B19" s="13">
         <v>0</v>
       </c>
-      <c r="C19" s="8">
-        <v>0</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="8">
-        <v>0</v>
-      </c>
-      <c r="G19" s="8">
-        <v>0</v>
-      </c>
-      <c r="H19" s="8">
+      <c r="C19" s="22">
+        <v>0</v>
+      </c>
+      <c r="D19" s="22">
+        <v>0</v>
+      </c>
+      <c r="E19" s="22">
+        <v>0</v>
+      </c>
+      <c r="F19" s="22">
+        <v>0</v>
+      </c>
+      <c r="G19" s="22">
+        <v>0</v>
+      </c>
+      <c r="H19" s="22">
         <v>1</v>
       </c>
       <c r="I19" s="8" t="s">
@@ -1799,22 +1820,22 @@
       <c r="B20" s="13">
         <v>0</v>
       </c>
-      <c r="C20" s="8">
-        <v>0</v>
-      </c>
-      <c r="D20" s="8">
-        <v>0</v>
-      </c>
-      <c r="E20" s="8">
-        <v>0</v>
-      </c>
-      <c r="F20" s="8">
-        <v>0</v>
-      </c>
-      <c r="G20" s="8">
-        <v>1</v>
-      </c>
-      <c r="H20" s="8">
+      <c r="C20" s="22">
+        <v>0</v>
+      </c>
+      <c r="D20" s="22">
+        <v>0</v>
+      </c>
+      <c r="E20" s="22">
+        <v>0</v>
+      </c>
+      <c r="F20" s="22">
+        <v>0</v>
+      </c>
+      <c r="G20" s="22">
+        <v>1</v>
+      </c>
+      <c r="H20" s="22">
         <v>0</v>
       </c>
       <c r="I20" s="8" t="s">
@@ -1855,22 +1876,22 @@
       <c r="B21" s="13">
         <v>0</v>
       </c>
-      <c r="C21" s="8">
-        <v>0</v>
-      </c>
-      <c r="D21" s="8">
-        <v>0</v>
-      </c>
-      <c r="E21" s="8">
-        <v>0</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0</v>
-      </c>
-      <c r="G21" s="8">
-        <v>1</v>
-      </c>
-      <c r="H21" s="8">
+      <c r="C21" s="22">
+        <v>0</v>
+      </c>
+      <c r="D21" s="22">
+        <v>0</v>
+      </c>
+      <c r="E21" s="22">
+        <v>0</v>
+      </c>
+      <c r="F21" s="22">
+        <v>0</v>
+      </c>
+      <c r="G21" s="22">
+        <v>1</v>
+      </c>
+      <c r="H21" s="22">
         <v>1</v>
       </c>
       <c r="I21" s="8" t="s">
@@ -1911,22 +1932,22 @@
       <c r="B22" s="13">
         <v>0</v>
       </c>
-      <c r="C22" s="8">
-        <v>0</v>
-      </c>
-      <c r="D22" s="8">
-        <v>0</v>
-      </c>
-      <c r="E22" s="8">
-        <v>0</v>
-      </c>
-      <c r="F22" s="8">
-        <v>1</v>
-      </c>
-      <c r="G22" s="8">
-        <v>0</v>
-      </c>
-      <c r="H22" s="8">
+      <c r="C22" s="22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="22">
+        <v>0</v>
+      </c>
+      <c r="H22" s="22">
         <v>0</v>
       </c>
       <c r="I22" s="8" t="s">
@@ -1967,22 +1988,22 @@
       <c r="B23" s="13">
         <v>0</v>
       </c>
-      <c r="C23" s="8">
-        <v>0</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0</v>
-      </c>
-      <c r="E23" s="8">
-        <v>0</v>
-      </c>
-      <c r="F23" s="8">
-        <v>1</v>
-      </c>
-      <c r="G23" s="8">
-        <v>0</v>
-      </c>
-      <c r="H23" s="8">
+      <c r="C23" s="22">
+        <v>0</v>
+      </c>
+      <c r="D23" s="22">
+        <v>0</v>
+      </c>
+      <c r="E23" s="22">
+        <v>0</v>
+      </c>
+      <c r="F23" s="22">
+        <v>1</v>
+      </c>
+      <c r="G23" s="22">
+        <v>0</v>
+      </c>
+      <c r="H23" s="22">
         <v>1</v>
       </c>
       <c r="I23" s="8" t="s">
@@ -2023,22 +2044,22 @@
       <c r="B24" s="13">
         <v>0</v>
       </c>
-      <c r="C24" s="8">
-        <v>0</v>
-      </c>
-      <c r="D24" s="8">
-        <v>0</v>
-      </c>
-      <c r="E24" s="8">
-        <v>0</v>
-      </c>
-      <c r="F24" s="8">
-        <v>1</v>
-      </c>
-      <c r="G24" s="8">
-        <v>1</v>
-      </c>
-      <c r="H24" s="8">
+      <c r="C24" s="22">
+        <v>0</v>
+      </c>
+      <c r="D24" s="22">
+        <v>0</v>
+      </c>
+      <c r="E24" s="22">
+        <v>0</v>
+      </c>
+      <c r="F24" s="22">
+        <v>1</v>
+      </c>
+      <c r="G24" s="22">
+        <v>1</v>
+      </c>
+      <c r="H24" s="22">
         <v>0</v>
       </c>
       <c r="I24" s="8" t="s">
@@ -2079,22 +2100,22 @@
       <c r="B25" s="13">
         <v>0</v>
       </c>
-      <c r="C25" s="8">
-        <v>0</v>
-      </c>
-      <c r="D25" s="8">
-        <v>0</v>
-      </c>
-      <c r="E25" s="8">
-        <v>0</v>
-      </c>
-      <c r="F25" s="8">
-        <v>1</v>
-      </c>
-      <c r="G25" s="8">
-        <v>1</v>
-      </c>
-      <c r="H25" s="8">
+      <c r="C25" s="22">
+        <v>0</v>
+      </c>
+      <c r="D25" s="22">
+        <v>0</v>
+      </c>
+      <c r="E25" s="22">
+        <v>0</v>
+      </c>
+      <c r="F25" s="22">
+        <v>1</v>
+      </c>
+      <c r="G25" s="22">
+        <v>1</v>
+      </c>
+      <c r="H25" s="22">
         <v>1</v>
       </c>
       <c r="I25" s="8" t="s">
@@ -2135,22 +2156,22 @@
       <c r="B26" s="13">
         <v>0</v>
       </c>
-      <c r="C26" s="8">
-        <v>0</v>
-      </c>
-      <c r="D26" s="8">
-        <v>0</v>
-      </c>
-      <c r="E26" s="8">
-        <v>1</v>
-      </c>
-      <c r="F26" s="8">
-        <v>0</v>
-      </c>
-      <c r="G26" s="8">
-        <v>0</v>
-      </c>
-      <c r="H26" s="8">
+      <c r="C26" s="22">
+        <v>0</v>
+      </c>
+      <c r="D26" s="22">
+        <v>0</v>
+      </c>
+      <c r="E26" s="22">
+        <v>1</v>
+      </c>
+      <c r="F26" s="22">
+        <v>0</v>
+      </c>
+      <c r="G26" s="22">
+        <v>0</v>
+      </c>
+      <c r="H26" s="22">
         <v>0</v>
       </c>
       <c r="I26" s="8" t="s">
@@ -2197,22 +2218,22 @@
       <c r="B29" s="12">
         <v>1</v>
       </c>
-      <c r="C29" s="2">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0</v>
-      </c>
-      <c r="H29" s="2">
+      <c r="C29" s="22">
+        <v>0</v>
+      </c>
+      <c r="D29" s="22">
+        <v>0</v>
+      </c>
+      <c r="E29" s="22">
+        <v>0</v>
+      </c>
+      <c r="F29" s="22">
+        <v>0</v>
+      </c>
+      <c r="G29" s="22">
+        <v>0</v>
+      </c>
+      <c r="H29" s="22">
         <v>1</v>
       </c>
       <c r="I29" s="4" t="s">
@@ -2253,22 +2274,22 @@
       <c r="B30" s="12">
         <v>1</v>
       </c>
-      <c r="C30" s="2">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
-      <c r="H30" s="2">
+      <c r="C30" s="22">
+        <v>0</v>
+      </c>
+      <c r="D30" s="22">
+        <v>0</v>
+      </c>
+      <c r="E30" s="22">
+        <v>0</v>
+      </c>
+      <c r="F30" s="22">
+        <v>0</v>
+      </c>
+      <c r="G30" s="22">
+        <v>1</v>
+      </c>
+      <c r="H30" s="22">
         <v>0</v>
       </c>
       <c r="I30" s="4" t="s">

</xml_diff>